<commit_message>
most of mini run
</commit_message>
<xml_diff>
--- a/2025-03-03_4o-mini_feedback_sheets/diff_gen/CREST syndrome with Type 2 Achalasia_vs_Esophageal stricture.xlsx
+++ b/2025-03-03_4o-mini_feedback_sheets/diff_gen/CREST syndrome with Type 2 Achalasia_vs_Esophageal stricture.xlsx
@@ -467,17 +467,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>These skin manifestations are characteristic of CREST syndrome and are not typically seen in esophageal stricture.</t>
+          <t>These findings are characteristic of CREST syndrome and are not typically associated with esophageal stricture.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Recent history of severe heartburn or regurgitation</t>
+          <t>Sudden onset of severe dysphagia</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>These symptoms are more commonly associated with esophageal stricture due to reflux or obstruction.</t>
+          <t>Sudden onset is more characteristic of esophageal stricture, which can occur due to acute processes.</t>
         </is>
       </c>
     </row>
@@ -489,17 +489,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Raynaud's phenomenon is a common feature of CREST syndrome and is not associated with esophageal stricture.</t>
+          <t>Raynaud's phenomenon is a common feature of CREST syndrome and is not seen in esophageal stricture.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Intermittent episodes of food getting stuck in the throat</t>
+          <t>History of recent weight loss without other systemic symptoms</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>This symptom is more typical of esophageal stricture, where obstruction leads to food impaction.</t>
+          <t>Weight loss without systemic symptoms is more indicative of esophageal stricture rather than the systemic features of CREST syndrome.</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>History of prior esophageal surgery or radiation</t>
+          <t>Presence of food impaction</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Prior interventions can lead to strictures, making this history more indicative of esophageal stricture.</t>
+          <t>Food impaction is more commonly reported in esophageal stricture due to narrowing of the esophagus.</t>
         </is>
       </c>
     </row>
@@ -538,12 +538,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Acute onset of dysphagia</t>
+          <t>History of prior esophageal surgery or radiation</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Acute dysphagia is more suggestive of esophageal stricture rather than the gradual onset seen in achalasia.</t>
+          <t>Prior interventions can lead to strictures, which is not a feature of CREST syndrome.</t>
         </is>
       </c>
     </row>
@@ -555,17 +555,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pulmonary hypertension is a systemic complication of CREST syndrome and is not a feature of esophageal stricture.</t>
+          <t>Pulmonary hypertension is associated with CREST syndrome and is not a feature of esophageal stricture.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Presence of odynophagia (painful swallowing)</t>
+          <t>Localized chest pain during swallowing</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Odynophagia is more commonly associated with esophageal stricture due to inflammation or ulceration.</t>
+          <t>Localized pain during swallowing is more typical of esophageal stricture than the diffuse symptoms seen in achalasia.</t>
         </is>
       </c>
     </row>
@@ -613,44 +613,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>History of sclerodactyly</t>
+          <t>History of scleroderma or related connective tissue disease</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sclerodactyly is a hallmark feature of CREST syndrome, which is not typically associated with esophageal stricture.</t>
+          <t>CREST syndrome is a subset of scleroderma, and a history of scleroderma strongly supports this diagnosis.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>History of chronic gastroesophageal reflux disease (GERD)</t>
+          <t>History of chronic gastroesophageal reflux disease</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GERD is a common precursor to esophageal stricture, while it is not a feature of CREST syndrome.</t>
+          <t>Chronic GERD is a common cause of esophageal stricture, making it a strong indicator for this diagnosis.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>History of Raynaud's phenomenon</t>
+          <t>Previous diagnosis of Raynaud's phenomenon</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Raynaud's phenomenon is commonly seen in CREST syndrome and is not a feature of esophageal stricture.</t>
+          <t>Raynaud's phenomenon is commonly associated with CREST syndrome, indicating a higher likelihood of this diagnosis.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>History of previous esophageal dilation procedures</t>
+          <t>Previous esophageal surgery for stricture repair</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Previous dilation is often performed for esophageal stricture, indicating a history of obstruction.</t>
+          <t>A history of surgical intervention for esophageal stricture directly supports the diagnosis of esophageal stricture.</t>
         </is>
       </c>
     </row>
@@ -662,61 +662,61 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pulmonary hypertension is associated with CREST syndrome and less commonly seen in esophageal stricture.</t>
+          <t>Pulmonary hypertension is a known complication of CREST syndrome, making it more likely in affected individuals.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>History of radiation therapy to the chest</t>
+          <t>Use of medications for strictures, such as corticosteroids</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Radiation therapy can lead to esophageal stricture, which is not related to CREST syndrome.</t>
+          <t>Corticosteroids may be used to manage inflammation in esophageal strictures, indicating this diagnosis.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>History of gastrointestinal motility disorders</t>
+          <t>Previous esophageal dilation procedures</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Gastrointestinal motility disorders are prevalent in CREST syndrome due to smooth muscle involvement, unlike esophageal stricture.</t>
+          <t>Patients with Type 2 Achalasia often undergo esophageal dilation, which may not be as common in esophageal stricture cases.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>History of ingestion of caustic substances</t>
+          <t>History of radiation therapy to the chest</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Ingestion of caustic substances can cause esophageal stricture, a condition not associated with CREST syndrome.</t>
+          <t>Radiation therapy can lead to esophageal strictures, making this a relevant finding for the diagnosis.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>History of skin changes (e.g., calcinosis)</t>
+          <t>Use of proton pump inhibitors for GERD management</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Calcinosis is a specific manifestation of CREST syndrome and not typically found in esophageal stricture.</t>
+          <t>GERD (Gastroesophageal Reflux Disease) is often treated in CREST syndrome patients due to esophageal motility issues.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>History of esophageal cancer</t>
+          <t>History of caustic ingestion</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Esophageal cancer can lead to strictures and is not a feature of CREST syndrome.</t>
+          <t>Caustic ingestion is a known cause of esophageal stricture, providing strong evidence for this diagnosis.</t>
         </is>
       </c>
     </row>
@@ -774,12 +774,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>History of gastroesophageal reflux disease (GERD)</t>
+          <t>History of chronic gastroesophageal reflux disease (GERD)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GERD is a common precursor to esophageal stricture, indicating a higher likelihood of this diagnosis.</t>
+          <t>GERD is a common risk factor for esophageal stricture, indicating a higher likelihood of this diagnosis.</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Raynaud's is a common feature of CREST syndrome, indicating a higher likelihood of this diagnosis.</t>
+          <t>Raynaud's phenomenon is a common feature of CREST syndrome, indicating a higher likelihood of this diagnosis.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>A genetic predisposition to esophageal cancer may correlate with the development of esophageal strictures.</t>
+          <t>A family history of esophageal cancer may suggest a predisposition to esophageal strictures.</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Certain exposures may increase the risk of autoimmune diseases like CREST syndrome.</t>
+          <t>Certain environmental exposures may increase the risk of autoimmune diseases like CREST syndrome.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Smoking is a known risk factor for esophageal strictures and related conditions.</t>
+          <t>Smoking is a known risk factor for esophageal strictures and related complications.</t>
         </is>
       </c>
     </row>
@@ -835,17 +835,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sclerodactyly is a hallmark of CREST syndrome, distinguishing it from esophageal stricture.</t>
+          <t>Sclerodactyly is a hallmark of CREST syndrome, which is less common in esophageal stricture.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>History of chronic alcohol use</t>
+          <t>History of heavy alcohol use</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Chronic alcohol use can lead to esophageal damage and strictures, favoring this diagnosis.</t>
+          <t>Heavy alcohol consumption can lead to esophageal damage and strictures.</t>
         </is>
       </c>
     </row>
@@ -867,7 +867,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Prior surgeries can lead to scarring and strictures, making esophageal stricture more likely.</t>
+          <t>Prior surgeries can lead to scarring and strictures in the esophagus.</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Weight loss is more commonly associated with esophageal stricture due to difficulty eating.</t>
+          <t>Weight loss is more commonly associated with esophageal stricture due to difficulty swallowing.</t>
         </is>
       </c>
     </row>
@@ -952,7 +952,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Odynophagia is more characteristic of esophageal stricture than of achalasia.</t>
+          <t>Odynophagia is a common symptom of esophageal stricture and less common in CREST syndrome with achalasia.</t>
         </is>
       </c>
     </row>
@@ -964,17 +964,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pulmonary hypertension can occur in CREST syndrome and is not a feature of esophageal stricture.</t>
+          <t>Pulmonary hypertension can occur in CREST syndrome and is not a typical finding in esophageal stricture.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Localized tenderness in the chest</t>
+          <t>Signs of malnutrition</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Localized tenderness may indicate an esophageal stricture, which can cause inflammation.</t>
+          <t>Malnutrition can occur due to prolonged dysphagia in esophageal stricture, unlike in CREST syndrome.</t>
         </is>
       </c>
     </row>
@@ -986,17 +986,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dysphagia with regurgitation is more characteristic of achalasia in CREST syndrome than esophageal stricture.</t>
+          <t>Dysphagia with regurgitation is more characteristic of achalasia in CREST syndrome than in esophageal stricture.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Normal skin examination</t>
+          <t>Localized tenderness in the chest</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>A normal skin examination would argue against CREST syndrome, which typically presents with skin changes.</t>
+          <t>Localized tenderness may indicate esophageal stricture, which can cause inflammation or irritation.</t>
         </is>
       </c>
     </row>
@@ -1008,17 +1008,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Esophageal dilation is indicative of achalasia, which is part of CREST syndrome, and not typically seen in esophageal stricture.</t>
+          <t>Esophageal dilation is indicative of achalasia, which is present in CREST syndrome but not in esophageal stricture.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>No signs of systemic sclerosis</t>
+          <t>Normal skin findings</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Absence of systemic sclerosis signs would favor esophageal stricture over CREST syndrome.</t>
+          <t>Normal skin findings are more indicative of esophageal stricture, as CREST syndrome typically presents with skin changes.</t>
         </is>
       </c>
     </row>
@@ -1076,12 +1076,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Barium swallow study showing localized narrowing or stricture</t>
+          <t>Barium swallow study showing a focal narrowing of the esophagus</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Localized narrowing is indicative of esophageal stricture, which is not seen in achalasia.</t>
+          <t>Focal narrowing is indicative of an esophageal stricture, which is not seen in achalasia.</t>
         </is>
       </c>
     </row>
@@ -1098,12 +1098,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Endoscopic findings showing a visible stricture with obstruction</t>
+          <t>Endoscopic findings revealing irregular, ulcerated mucosa</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Visible obstruction is a key feature of esophageal stricture, distinguishing it from achalasia.</t>
+          <t>Irregular and ulcerated mucosa is more consistent with esophageal stricture than with achalasia.</t>
         </is>
       </c>
     </row>
@@ -1115,61 +1115,61 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The 'bird-beak' sign is indicative of achalasia, which is more common in CREST syndrome.</t>
+          <t>The 'bird-beak' appearance on imaging is indicative of achalasia, which is more common in CREST syndrome.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Histological examination showing fibrosis or inflammation</t>
+          <t>CT scan showing a mass or lesion causing obstruction</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fibrosis or inflammation is more typical of esophageal stricture than achalasia.</t>
+          <t>A mass or lesion on imaging suggests a stricture rather than the motility disorder seen in achalasia.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Endoscopic findings showing esophageal dilation without obstruction</t>
+          <t>Presence of esophageal dilation on CT scan</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dilation without obstruction aligns with achalasia rather than strictures, favoring CREST syndrome.</t>
+          <t>Esophageal dilation is more frequently observed in patients with achalasia than in those with strictures.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Esophageal imaging showing irregularities in the esophageal wall</t>
+          <t>Esophageal biopsy showing dysplasia or malignancy</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Irregularities in the wall are more consistent with strictures than with achalasia.</t>
+          <t>Dysplasia or malignancy is more commonly associated with strictures than with achalasia.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Presence of anti-centromere antibodies in serological tests</t>
+          <t>Endoscopic findings showing normal mucosa with significant dilation</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anti-centromere antibodies are often present in CREST syndrome, supporting its diagnosis.</t>
+          <t>Normal mucosal appearance with dilation suggests achalasia rather than a stricture, favoring CREST syndrome.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Presence of esophageal ulcers or lesions on endoscopy</t>
+          <t>Esophageal manometry showing normal LES pressure</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ulcers or lesions are more commonly associated with esophageal strictures.</t>
+          <t>Normal LES pressure is inconsistent with achalasia and supports the diagnosis of esophageal stricture.</t>
         </is>
       </c>
     </row>

</xml_diff>